<commit_message>
typo (Cladospiorium -> Cladosporium)
</commit_message>
<xml_diff>
--- a/Data/data_sour_rot.xlsx
+++ b/Data/data_sour_rot.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Seb\Desktop\article communauté dernière version\final\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\U80821784\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6EF4E16F-B3D6-4338-A06F-851797690BC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCB6EEBB-3319-42A9-85A1-5EC68D1651C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -384,9 +384,6 @@
     <t xml:space="preserve">Chaetomium </t>
   </si>
   <si>
-    <t>Cladospiorium</t>
-  </si>
-  <si>
     <t xml:space="preserve">Cladosporium </t>
   </si>
   <si>
@@ -1172,6 +1169,9 @@
   </si>
   <si>
     <t>Pichia kurdriavzevii</t>
+  </si>
+  <si>
+    <t>Cladosporium</t>
   </si>
 </sst>
 </file>
@@ -2571,7 +2571,7 @@
   <dimension ref="A1:DY139"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A95" sqref="A95"/>
+      <selection activeCell="A18" sqref="A18:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2584,7 +2584,7 @@
   <sheetData>
     <row r="1" spans="1:129" x14ac:dyDescent="0.25">
       <c r="E1" s="18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F1" s="18"/>
       <c r="G1" s="18"/>
@@ -2626,7 +2626,7 @@
       <c r="AQ1" s="18"/>
       <c r="AR1" s="18"/>
       <c r="AS1" s="18" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="AT1" s="18"/>
       <c r="AU1" s="18"/>
@@ -2695,7 +2695,7 @@
       <c r="DF1" s="18"/>
       <c r="DG1" s="18"/>
       <c r="DH1" s="18" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="DI1" s="18"/>
       <c r="DJ1" s="18"/>
@@ -2720,10 +2720,10 @@
         <v>108</v>
       </c>
       <c r="B2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D2" s="11" t="s">
         <v>109</v>
@@ -3050,72 +3050,72 @@
         <v>106</v>
       </c>
       <c r="DH2" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="DI2" s="7" t="s">
         <v>205</v>
       </c>
-      <c r="DI2" s="7" t="s">
+      <c r="DJ2" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="DJ2" s="7" t="s">
+      <c r="DK2" s="7" t="s">
         <v>207</v>
       </c>
-      <c r="DK2" s="7" t="s">
+      <c r="DL2" s="7" t="s">
         <v>208</v>
       </c>
-      <c r="DL2" s="7" t="s">
+      <c r="DM2" s="7" t="s">
         <v>209</v>
       </c>
-      <c r="DM2" s="7" t="s">
+      <c r="DN2" s="12" t="s">
         <v>210</v>
       </c>
-      <c r="DN2" s="12" t="s">
+      <c r="DO2" s="12" t="s">
         <v>211</v>
       </c>
-      <c r="DO2" s="12" t="s">
+      <c r="DP2" s="12" t="s">
         <v>212</v>
       </c>
-      <c r="DP2" s="12" t="s">
+      <c r="DQ2" s="12" t="s">
         <v>213</v>
       </c>
-      <c r="DQ2" s="12" t="s">
+      <c r="DR2" s="12" t="s">
         <v>214</v>
       </c>
-      <c r="DR2" s="12" t="s">
+      <c r="DS2" s="13" t="s">
         <v>215</v>
       </c>
-      <c r="DS2" s="13" t="s">
+      <c r="DT2" s="12" t="s">
         <v>216</v>
       </c>
-      <c r="DT2" s="12" t="s">
+      <c r="DU2" s="12" t="s">
         <v>217</v>
       </c>
-      <c r="DU2" s="12" t="s">
+      <c r="DV2" s="12" t="s">
         <v>218</v>
       </c>
-      <c r="DV2" s="12" t="s">
+      <c r="DW2" s="12" t="s">
         <v>219</v>
       </c>
-      <c r="DW2" s="12" t="s">
+      <c r="DX2" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="DX2" s="12" t="s">
+      <c r="DY2" s="13" t="s">
         <v>221</v>
-      </c>
-      <c r="DY2" s="13" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="3" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>110</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E3">
         <v>4</v>
@@ -3258,16 +3258,16 @@
     </row>
     <row r="4" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>110</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AD4">
         <v>1</v>
@@ -3276,30 +3276,30 @@
     </row>
     <row r="5" spans="1:129" ht="18" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>111</v>
       </c>
       <c r="C5" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>162</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="6" spans="1:129" ht="18" x14ac:dyDescent="0.35">
       <c r="A6" s="9" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>112</v>
       </c>
       <c r="C6" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="D6" s="9" t="s">
         <v>164</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>165</v>
       </c>
       <c r="W6">
         <v>1</v>
@@ -3308,16 +3308,16 @@
     </row>
     <row r="7" spans="1:129" ht="18" x14ac:dyDescent="0.35">
       <c r="A7" s="8" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>113</v>
       </c>
       <c r="C7" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="D7" s="8" t="s">
         <v>164</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>165</v>
       </c>
       <c r="AZ7">
         <v>1</v>
@@ -3328,16 +3328,16 @@
     </row>
     <row r="8" spans="1:129" ht="18" x14ac:dyDescent="0.35">
       <c r="A8" s="9" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>113</v>
       </c>
       <c r="C8" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="D8" s="9" t="s">
         <v>164</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>165</v>
       </c>
       <c r="AS8" s="10"/>
       <c r="BH8">
@@ -3346,16 +3346,16 @@
     </row>
     <row r="9" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>114</v>
       </c>
       <c r="C9" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D9" s="8" t="s">
         <v>166</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>167</v>
       </c>
       <c r="E9">
         <v>3</v>
@@ -3441,45 +3441,45 @@
     </row>
     <row r="10" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>115</v>
       </c>
       <c r="C10" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="D10" s="9" t="s">
         <v>168</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>169</v>
       </c>
       <c r="AS10" s="10"/>
     </row>
     <row r="11" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>115</v>
       </c>
       <c r="C11" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="D11" s="8" t="s">
         <v>168</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="12" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B12" s="9" t="s">
         <v>116</v>
       </c>
       <c r="C12" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="D12" s="9" t="s">
         <v>170</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>171</v>
       </c>
       <c r="AS12" s="10"/>
       <c r="AU12">
@@ -3521,16 +3521,16 @@
     </row>
     <row r="13" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="AW13">
         <v>5</v>
@@ -3601,16 +3601,16 @@
     </row>
     <row r="14" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="AS14" s="10"/>
       <c r="CJ14">
@@ -3619,16 +3619,16 @@
     </row>
     <row r="15" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B15" s="8" t="s">
         <v>117</v>
       </c>
       <c r="C15" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="D15" s="8" t="s">
         <v>174</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>175</v>
       </c>
       <c r="AW15">
         <v>2</v>
@@ -3651,16 +3651,16 @@
     </row>
     <row r="16" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B16" s="9" t="s">
         <v>117</v>
       </c>
       <c r="C16" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="D16" s="9" t="s">
         <v>174</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>175</v>
       </c>
       <c r="AS16" s="10"/>
       <c r="BM16">
@@ -3672,16 +3672,16 @@
     </row>
     <row r="17" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>118</v>
       </c>
       <c r="C17" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="D17" s="8" t="s">
         <v>176</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>177</v>
       </c>
       <c r="DN17">
         <v>1</v>
@@ -3689,16 +3689,16 @@
     </row>
     <row r="18" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>119</v>
+        <v>374</v>
       </c>
       <c r="C18" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="D18" s="9" t="s">
         <v>178</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>179</v>
       </c>
       <c r="H18">
         <v>1</v>
@@ -3749,16 +3749,16 @@
     </row>
     <row r="19" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C19" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="D19" s="8" t="s">
         <v>178</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>179</v>
       </c>
       <c r="AK19">
         <v>1</v>
@@ -3766,16 +3766,16 @@
     </row>
     <row r="20" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C20" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="D20" s="9" t="s">
         <v>178</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>179</v>
       </c>
       <c r="AP20">
         <v>1</v>
@@ -3790,30 +3790,30 @@
     </row>
     <row r="21" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C21" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="D21" s="8" t="s">
         <v>180</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="22" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="AE22">
         <v>1</v>
@@ -3831,16 +3831,16 @@
     </row>
     <row r="23" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F23">
         <v>1</v>
@@ -3848,60 +3848,60 @@
     </row>
     <row r="24" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="AS24" s="10"/>
     </row>
     <row r="25" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="26" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AS26" s="10"/>
     </row>
     <row r="27" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="DY27">
         <v>1</v>
@@ -3909,16 +3909,16 @@
     </row>
     <row r="28" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="X28">
         <v>1</v>
@@ -3930,16 +3930,16 @@
     </row>
     <row r="29" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F29">
         <v>1</v>
@@ -3959,16 +3959,16 @@
     </row>
     <row r="30" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C30" s="15" t="s">
+        <v>359</v>
+      </c>
+      <c r="D30" s="15" t="s">
         <v>360</v>
-      </c>
-      <c r="D30" s="15" t="s">
-        <v>361</v>
       </c>
       <c r="M30">
         <v>1</v>
@@ -4010,16 +4010,16 @@
     </row>
     <row r="31" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C31" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="D31" s="8" t="s">
         <v>186</v>
-      </c>
-      <c r="D31" s="8" t="s">
-        <v>187</v>
       </c>
       <c r="BV31">
         <v>1</v>
@@ -4027,16 +4027,16 @@
     </row>
     <row r="32" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C32" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="D32" s="9" t="s">
         <v>186</v>
-      </c>
-      <c r="D32" s="9" t="s">
-        <v>187</v>
       </c>
       <c r="L32">
         <v>1</v>
@@ -4045,16 +4045,16 @@
     </row>
     <row r="33" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C33" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="D33" s="8" t="s">
         <v>186</v>
-      </c>
-      <c r="D33" s="8" t="s">
-        <v>187</v>
       </c>
       <c r="J33">
         <v>1</v>
@@ -4062,16 +4062,16 @@
     </row>
     <row r="34" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="AS34" s="10"/>
       <c r="CO34">
@@ -4092,16 +4092,16 @@
     </row>
     <row r="35" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="DB35">
         <v>1</v>
@@ -4112,16 +4112,16 @@
     </row>
     <row r="36" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="M36">
         <v>1</v>
@@ -4133,16 +4133,16 @@
     </row>
     <row r="37" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="DL37">
         <v>5</v>
@@ -4156,16 +4156,16 @@
     </row>
     <row r="38" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="AS38" s="10"/>
       <c r="CJ38">
@@ -4180,16 +4180,16 @@
     </row>
     <row r="39" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="BM39">
         <v>2</v>
@@ -4221,16 +4221,16 @@
     </row>
     <row r="40" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="AS40" s="10"/>
       <c r="DO40">
@@ -4239,16 +4239,16 @@
     </row>
     <row r="41" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F41">
         <v>1</v>
@@ -4355,16 +4355,16 @@
     </row>
     <row r="42" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="AS42" s="10"/>
       <c r="BM42">
@@ -4382,16 +4382,16 @@
     </row>
     <row r="43" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A43" s="8" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="X43">
         <v>1</v>
@@ -4423,16 +4423,16 @@
     </row>
     <row r="44" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="AS44" s="10"/>
       <c r="BB44">
@@ -4447,16 +4447,16 @@
     </row>
     <row r="45" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A45" s="8" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="AU45">
         <v>1</v>
@@ -4476,16 +4476,16 @@
     </row>
     <row r="46" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A46" s="9" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D46" s="9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="L46">
         <v>1</v>
@@ -4509,16 +4509,16 @@
     </row>
     <row r="47" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A47" s="8" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="CF47">
         <v>2</v>
@@ -4541,16 +4541,16 @@
     </row>
     <row r="48" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A48" s="9" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D48" s="9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="AS48" s="10"/>
       <c r="DD48">
@@ -4559,16 +4559,16 @@
     </row>
     <row r="49" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A49" s="8" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="CI49">
         <v>1</v>
@@ -4576,16 +4576,16 @@
     </row>
     <row r="50" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A50" s="9" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D50" s="9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="M50">
         <v>1</v>
@@ -4597,16 +4597,16 @@
     </row>
     <row r="51" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A51" s="8" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="O51">
         <v>1</v>
@@ -4647,16 +4647,16 @@
     </row>
     <row r="52" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A52" s="9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D52" s="9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H52">
         <v>1</v>
@@ -4779,16 +4779,16 @@
     </row>
     <row r="53" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A53" s="8" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="AI53">
         <v>1</v>
@@ -4817,16 +4817,16 @@
     </row>
     <row r="54" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A54" s="9" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D54" s="9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="K54">
         <v>1</v>
@@ -4901,16 +4901,16 @@
     </row>
     <row r="55" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A55" s="8" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="R55">
         <v>1</v>
@@ -4945,16 +4945,16 @@
     </row>
     <row r="56" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D56" s="9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="AS56" s="10"/>
       <c r="DY56">
@@ -4963,16 +4963,16 @@
     </row>
     <row r="57" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A57" s="8" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F57">
         <v>2</v>
@@ -5106,31 +5106,31 @@
     </row>
     <row r="58" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A58" s="9" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D58" s="9" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="AS58" s="10"/>
     </row>
     <row r="59" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A59" s="8" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C59" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="D59" s="8" t="s">
         <v>188</v>
-      </c>
-      <c r="D59" s="8" t="s">
-        <v>189</v>
       </c>
       <c r="G59">
         <v>1</v>
@@ -5147,16 +5147,16 @@
     </row>
     <row r="60" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A60" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D60" s="9" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AS60" s="10"/>
       <c r="DK60">
@@ -5165,16 +5165,16 @@
     </row>
     <row r="61" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A61" s="8" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B61" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="C61" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="C61" s="8" t="s">
-        <v>139</v>
-      </c>
       <c r="D61" s="8" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E61">
         <v>1</v>
@@ -5182,16 +5182,16 @@
     </row>
     <row r="62" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A62" s="9" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B62" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="C62" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="C62" s="9" t="s">
-        <v>139</v>
-      </c>
       <c r="D62" s="9" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="N62">
         <v>1</v>
@@ -5206,16 +5206,16 @@
     </row>
     <row r="63" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A63" s="8" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B63" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="C63" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="C63" s="8" t="s">
-        <v>139</v>
-      </c>
       <c r="D63" s="8" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="R63">
         <v>1</v>
@@ -5226,16 +5226,16 @@
     </row>
     <row r="64" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A64" s="9" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B64" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="C64" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="C64" s="9" t="s">
-        <v>139</v>
-      </c>
       <c r="D64" s="9" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="AS64" s="10"/>
       <c r="CG64">
@@ -5247,16 +5247,16 @@
     </row>
     <row r="65" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A65" s="8" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B65" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="C65" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="C65" s="8" t="s">
-        <v>139</v>
-      </c>
       <c r="D65" s="8" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="AU65">
         <v>1</v>
@@ -5264,16 +5264,16 @@
     </row>
     <row r="66" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A66" s="9" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B66" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="C66" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="C66" s="9" t="s">
-        <v>139</v>
-      </c>
       <c r="D66" s="9" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="O66">
         <v>1</v>
@@ -5294,16 +5294,16 @@
     </row>
     <row r="67" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A67" s="8" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B67" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="C67" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="C67" s="8" t="s">
-        <v>139</v>
-      </c>
       <c r="D67" s="8" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="AB67">
         <v>2</v>
@@ -5311,16 +5311,16 @@
     </row>
     <row r="68" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A68" s="9" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B68" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="C68" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="C68" s="9" t="s">
-        <v>139</v>
-      </c>
       <c r="D68" s="9" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="M68">
         <v>1</v>
@@ -5347,16 +5347,16 @@
     </row>
     <row r="69" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A69" s="8" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B69" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="C69" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="C69" s="8" t="s">
-        <v>139</v>
-      </c>
       <c r="D69" s="8" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="X69">
         <v>1</v>
@@ -5367,16 +5367,16 @@
     </row>
     <row r="70" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A70" s="9" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B70" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="C70" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="C70" s="9" t="s">
-        <v>139</v>
-      </c>
       <c r="D70" s="9" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="AO70">
         <v>1</v>
@@ -5385,16 +5385,16 @@
     </row>
     <row r="71" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A71" s="8" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B71" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="C71" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="C71" s="8" t="s">
-        <v>139</v>
-      </c>
       <c r="D71" s="8" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="CT71">
         <v>1</v>
@@ -5405,16 +5405,16 @@
     </row>
     <row r="72" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A72" s="9" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B72" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="C72" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="C72" s="9" t="s">
-        <v>139</v>
-      </c>
       <c r="D72" s="9" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="Q72">
         <v>1</v>
@@ -5432,16 +5432,16 @@
     </row>
     <row r="73" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A73" s="8" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B73" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C73" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="D73" s="8" t="s">
         <v>191</v>
-      </c>
-      <c r="D73" s="8" t="s">
-        <v>192</v>
       </c>
       <c r="CS73">
         <v>1</v>
@@ -5455,16 +5455,16 @@
     </row>
     <row r="74" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A74" s="9" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B74" s="9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C74" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="D74" s="9" t="s">
         <v>191</v>
-      </c>
-      <c r="D74" s="9" t="s">
-        <v>192</v>
       </c>
       <c r="AS74" s="10"/>
       <c r="DS74">
@@ -5473,16 +5473,16 @@
     </row>
     <row r="75" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A75" s="8" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B75" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C75" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="D75" s="8" t="s">
         <v>191</v>
-      </c>
-      <c r="D75" s="8" t="s">
-        <v>192</v>
       </c>
       <c r="BU75">
         <v>1</v>
@@ -5496,60 +5496,60 @@
     </row>
     <row r="76" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A76" s="9" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B76" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C76" s="9" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D76" s="9" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="AS76" s="10"/>
     </row>
     <row r="77" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A77" s="8" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B77" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C77" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D77" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="78" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A78" s="9" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B78" s="9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C78" s="9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D78" s="9" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="AS78" s="10"/>
     </row>
     <row r="79" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A79" s="8" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B79" s="8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C79" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D79" s="8" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="DI79">
         <v>1</v>
@@ -5557,16 +5557,16 @@
     </row>
     <row r="80" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A80" s="9" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B80" s="9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C80" s="9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D80" s="9" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="E80">
         <v>2</v>
@@ -5590,16 +5590,16 @@
     </row>
     <row r="81" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A81" s="8" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B81" s="8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C81" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D81" s="8" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="E81">
         <v>1</v>
@@ -5607,16 +5607,16 @@
     </row>
     <row r="82" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A82" s="9" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B82" s="9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C82" s="9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D82" s="9" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="AS82" s="10"/>
       <c r="DK82">
@@ -5625,16 +5625,16 @@
     </row>
     <row r="83" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A83" s="8" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B83" s="8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C83" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D83" s="8" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="CQ83">
         <v>2</v>
@@ -5666,16 +5666,16 @@
     </row>
     <row r="84" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A84" s="9" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B84" s="9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C84" s="9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D84" s="9" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="Z84">
         <v>1</v>
@@ -5684,16 +5684,16 @@
     </row>
     <row r="85" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A85" s="8" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B85" s="15" t="s">
+        <v>352</v>
+      </c>
+      <c r="C85" s="15" t="s">
         <v>353</v>
       </c>
-      <c r="C85" s="15" t="s">
-        <v>354</v>
-      </c>
       <c r="D85" s="8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="DT85">
         <v>1</v>
@@ -5701,16 +5701,16 @@
     </row>
     <row r="86" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A86" s="9" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B86" s="9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C86" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D86" s="9" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="S86">
         <v>1</v>
@@ -5740,16 +5740,16 @@
     </row>
     <row r="87" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A87" s="8" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B87" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C87" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D87" s="8" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="DC87">
         <v>1</v>
@@ -5757,16 +5757,16 @@
     </row>
     <row r="88" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A88" s="9" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B88" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C88" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D88" s="9" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="AS88" s="10"/>
       <c r="CJ88">
@@ -5787,16 +5787,16 @@
     </row>
     <row r="89" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A89" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B89" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C89" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D89" s="8" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="CI89">
         <v>1</v>
@@ -5810,16 +5810,16 @@
     </row>
     <row r="90" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A90" s="9" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B90" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C90" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D90" s="9" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="AS90" s="10"/>
       <c r="CQ90">
@@ -5828,16 +5828,16 @@
     </row>
     <row r="91" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A91" s="8" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B91" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C91" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D91" s="8" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="CT91">
         <v>1</v>
@@ -5845,16 +5845,16 @@
     </row>
     <row r="92" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A92" s="9" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B92" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C92" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D92" s="9" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="AS92" s="10"/>
       <c r="CC92">
@@ -5863,16 +5863,16 @@
     </row>
     <row r="93" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A93" s="8" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B93" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C93" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D93" s="8" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="BN93">
         <v>1</v>
@@ -5889,16 +5889,16 @@
     </row>
     <row r="94" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A94" s="9" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B94" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C94" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D94" s="9" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="AS94" s="10"/>
       <c r="CI94">
@@ -5913,16 +5913,16 @@
     </row>
     <row r="95" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A95" s="8" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B95" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C95" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D95" s="8" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="CA95">
         <v>1</v>
@@ -5936,16 +5936,16 @@
     </row>
     <row r="96" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A96" s="9" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B96" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C96" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D96" s="9" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="AS96" s="10"/>
       <c r="CW96">
@@ -5957,16 +5957,16 @@
     </row>
     <row r="97" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A97" s="8" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B97" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C97" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D97" s="8" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="M97">
         <v>1</v>
@@ -6019,16 +6019,16 @@
     </row>
     <row r="98" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A98" s="9" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B98" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C98" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D98" s="9" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="AS98" s="10"/>
       <c r="CY98">
@@ -6040,16 +6040,16 @@
     </row>
     <row r="99" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A99" s="8" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B99" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C99" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D99" s="8" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="DN99">
         <v>2</v>
@@ -6057,16 +6057,16 @@
     </row>
     <row r="100" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A100" s="9" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B100" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C100" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D100" s="9" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="AS100" s="10"/>
       <c r="BZ100">
@@ -6078,16 +6078,16 @@
     </row>
     <row r="101" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A101" s="8" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B101" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C101" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D101" s="8" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="BQ101">
         <v>1</v>
@@ -6104,16 +6104,16 @@
     </row>
     <row r="102" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A102" s="9" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B102" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C102" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D102" s="9" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="AS102" s="10"/>
       <c r="BP102">
@@ -6143,16 +6143,16 @@
     </row>
     <row r="103" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A103" s="8" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B103" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C103" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D103" s="8" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="CB103">
         <v>1</v>
@@ -6163,16 +6163,16 @@
     </row>
     <row r="104" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A104" s="9" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B104" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C104" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D104" s="9" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="S104">
         <v>1</v>
@@ -6226,16 +6226,16 @@
     </row>
     <row r="105" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A105" s="8" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B105" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C105" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D105" s="8" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="BS105">
         <v>1</v>
@@ -6243,16 +6243,16 @@
     </row>
     <row r="106" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A106" s="9" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B106" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C106" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D106" s="9" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="AS106" s="10"/>
       <c r="CE106">
@@ -6261,16 +6261,16 @@
     </row>
     <row r="107" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A107" s="8" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B107" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C107" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D107" s="8" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="F107">
         <v>1</v>
@@ -6302,16 +6302,16 @@
     </row>
     <row r="108" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A108" s="9" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B108" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C108" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D108" s="9" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="AS108" s="10"/>
       <c r="DI108">
@@ -6332,16 +6332,16 @@
     </row>
     <row r="109" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A109" s="8" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B109" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C109" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D109" s="8" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="J109">
         <v>1</v>
@@ -6349,16 +6349,16 @@
     </row>
     <row r="110" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A110" s="9" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B110" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C110" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D110" s="9" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="AS110" s="10"/>
       <c r="DN110">
@@ -6367,16 +6367,16 @@
     </row>
     <row r="111" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A111" s="8" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B111" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C111" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D111" s="8" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="CZ111">
         <v>1</v>
@@ -6387,16 +6387,16 @@
     </row>
     <row r="112" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A112" s="9" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B112" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C112" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D112" s="9" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="O112">
         <v>1</v>
@@ -6447,16 +6447,16 @@
     </row>
     <row r="113" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A113" s="8" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B113" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C113" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="D113" s="8" t="s">
         <v>172</v>
-      </c>
-      <c r="D113" s="8" t="s">
-        <v>173</v>
       </c>
       <c r="J113">
         <v>1</v>
@@ -6476,16 +6476,16 @@
     </row>
     <row r="114" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A114" s="9" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B114" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C114" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D114" s="9" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="AS114" s="10"/>
       <c r="CA114">
@@ -6506,16 +6506,16 @@
     </row>
     <row r="115" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A115" s="8" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B115" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C115" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="D115" s="8" t="s">
         <v>172</v>
-      </c>
-      <c r="D115" s="8" t="s">
-        <v>173</v>
       </c>
       <c r="BI115">
         <v>1</v>
@@ -6559,16 +6559,16 @@
     </row>
     <row r="116" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A116" s="9" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B116" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C116" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D116" s="9" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="AS116" s="10"/>
       <c r="DS116">
@@ -6577,16 +6577,16 @@
     </row>
     <row r="117" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A117" s="8" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B117" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C117" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D117" s="8" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="CU117">
         <v>1</v>
@@ -6603,16 +6603,16 @@
     </row>
     <row r="118" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A118" s="9" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B118" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C118" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D118" s="9" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="S118">
         <v>1</v>
@@ -6633,16 +6633,16 @@
     </row>
     <row r="119" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A119" s="8" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B119" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C119" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D119" s="8" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="CH119">
         <v>1</v>
@@ -6653,16 +6653,16 @@
     </row>
     <row r="120" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A120" s="9" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B120" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C120" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D120" s="9" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="AS120" s="10"/>
       <c r="CV120">
@@ -6674,16 +6674,16 @@
     </row>
     <row r="121" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A121" s="8" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B121" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C121" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D121" s="8" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="CH121">
         <v>1</v>
@@ -6697,16 +6697,16 @@
     </row>
     <row r="122" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A122" s="8" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B122" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C122" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D122" s="8" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="BK122">
         <v>2</v>
@@ -6765,16 +6765,16 @@
     </row>
     <row r="123" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A123" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B123" s="9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C123" s="9" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D123" s="9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AL123">
         <v>1</v>
@@ -6795,16 +6795,16 @@
     </row>
     <row r="124" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A124" s="8" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B124" s="8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C124" s="8" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="D124" s="8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AE124">
         <v>1</v>
@@ -6812,16 +6812,16 @@
     </row>
     <row r="125" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A125" s="9" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B125" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C125" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="D125" s="9" t="s">
         <v>194</v>
-      </c>
-      <c r="D125" s="9" t="s">
-        <v>195</v>
       </c>
       <c r="E125">
         <v>1</v>
@@ -6836,16 +6836,16 @@
     </row>
     <row r="126" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A126" s="8" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B126" s="8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C126" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="D126" s="8" t="s">
         <v>194</v>
-      </c>
-      <c r="D126" s="8" t="s">
-        <v>195</v>
       </c>
       <c r="J126">
         <v>1</v>
@@ -6856,13 +6856,13 @@
         <v>107</v>
       </c>
       <c r="B127" s="15" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C127" s="15" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D127" s="9" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="M127">
         <v>2</v>
@@ -6871,16 +6871,16 @@
     </row>
     <row r="128" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A128" s="8" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B128" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C128" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D128" s="8" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="DV128">
         <v>1</v>
@@ -6894,16 +6894,16 @@
     </row>
     <row r="129" spans="1:128" x14ac:dyDescent="0.25">
       <c r="A129" s="9" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B129" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C129" s="9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D129" s="9" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="AS129" s="10"/>
       <c r="DV129">
@@ -6912,16 +6912,16 @@
     </row>
     <row r="130" spans="1:128" x14ac:dyDescent="0.25">
       <c r="A130" s="8" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B130" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C130" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D130" s="8" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="CK130">
         <v>1</v>
@@ -6938,16 +6938,16 @@
     </row>
     <row r="131" spans="1:128" x14ac:dyDescent="0.25">
       <c r="A131" s="9" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B131" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C131" s="9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D131" s="9" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="S131">
         <v>4</v>
@@ -6965,16 +6965,16 @@
     </row>
     <row r="132" spans="1:128" x14ac:dyDescent="0.25">
       <c r="A132" s="8" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B132" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C132" s="8" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D132" s="8" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="K132">
         <v>1</v>
@@ -6982,31 +6982,31 @@
     </row>
     <row r="133" spans="1:128" x14ac:dyDescent="0.25">
       <c r="A133" s="9" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B133" s="15" t="s">
+        <v>356</v>
+      </c>
+      <c r="C133" s="15" t="s">
         <v>357</v>
       </c>
-      <c r="C133" s="15" t="s">
+      <c r="D133" s="15" t="s">
         <v>358</v>
-      </c>
-      <c r="D133" s="15" t="s">
-        <v>359</v>
       </c>
       <c r="AS133" s="10"/>
     </row>
     <row r="134" spans="1:128" x14ac:dyDescent="0.25">
       <c r="A134" s="8" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B134" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C134" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="D134" s="8" t="s">
         <v>194</v>
-      </c>
-      <c r="D134" s="8" t="s">
-        <v>195</v>
       </c>
       <c r="AL134">
         <v>1</v>
@@ -7014,16 +7014,16 @@
     </row>
     <row r="135" spans="1:128" x14ac:dyDescent="0.25">
       <c r="A135" s="9" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B135" s="9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C135" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="D135" s="9" t="s">
         <v>194</v>
-      </c>
-      <c r="D135" s="9" t="s">
-        <v>195</v>
       </c>
       <c r="J135">
         <v>1</v>
@@ -7035,16 +7035,16 @@
     </row>
     <row r="136" spans="1:128" x14ac:dyDescent="0.25">
       <c r="A136" s="8" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B136" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C136" s="14" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D136" s="8" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="AX136">
         <v>1</v>
@@ -7058,16 +7058,16 @@
     </row>
     <row r="137" spans="1:128" x14ac:dyDescent="0.25">
       <c r="A137" s="9" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B137" s="9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C137" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D137" s="9" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="Q137">
         <v>1</v>
@@ -7079,30 +7079,30 @@
     </row>
     <row r="138" spans="1:128" x14ac:dyDescent="0.25">
       <c r="A138" s="8" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B138" s="8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C138" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="D138" s="8" t="s">
         <v>168</v>
-      </c>
-      <c r="D138" s="8" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="139" spans="1:128" x14ac:dyDescent="0.25">
       <c r="A139" s="9" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B139" s="9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C139" s="9" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D139" s="9" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="AS139" s="10"/>
       <c r="BJ139">

</xml_diff>

<commit_message>
californica -> Pichia instead of Candida (update MycoBank)
</commit_message>
<xml_diff>
--- a/Data/data_sour_rot.xlsx
+++ b/Data/data_sour_rot.xlsx
@@ -8,17 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\U80821784\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCB6EEBB-3319-42A9-85A1-5EC68D1651C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{028BBA51-D238-4642-8A4F-A2CA22065A2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -745,9 +754,6 @@
     <t>Botrytis sp.</t>
   </si>
   <si>
-    <t>Candida californica</t>
-  </si>
-  <si>
     <t>Candida railenensis</t>
   </si>
   <si>
@@ -1172,6 +1178,9 @@
   </si>
   <si>
     <t>Cladosporium</t>
+  </si>
+  <si>
+    <t>Pichia californica</t>
   </si>
 </sst>
 </file>
@@ -2571,7 +2580,7 @@
   <dimension ref="A1:DY139"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:XFD18"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -3521,16 +3530,16 @@
     </row>
     <row r="13" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>232</v>
+        <v>374</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>131</v>
+        <v>144</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>171</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="AW13">
         <v>5</v>
@@ -3601,7 +3610,7 @@
     </row>
     <row r="14" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B14" s="9" t="s">
         <v>131</v>
@@ -3610,7 +3619,7 @@
         <v>171</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="AS14" s="10"/>
       <c r="CJ14">
@@ -3619,7 +3628,7 @@
     </row>
     <row r="15" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B15" s="8" t="s">
         <v>117</v>
@@ -3651,7 +3660,7 @@
     </row>
     <row r="16" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B16" s="9" t="s">
         <v>117</v>
@@ -3672,7 +3681,7 @@
     </row>
     <row r="17" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>118</v>
@@ -3689,10 +3698,10 @@
     </row>
     <row r="18" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>177</v>
@@ -3749,7 +3758,7 @@
     </row>
     <row r="19" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>119</v>
@@ -3766,7 +3775,7 @@
     </row>
     <row r="20" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B20" s="9" t="s">
         <v>119</v>
@@ -3790,7 +3799,7 @@
     </row>
     <row r="21" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>120</v>
@@ -3804,7 +3813,7 @@
     </row>
     <row r="22" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B22" s="9" t="s">
         <v>121</v>
@@ -3831,7 +3840,7 @@
     </row>
     <row r="23" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>122</v>
@@ -3848,7 +3857,7 @@
     </row>
     <row r="24" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B24" s="9" t="s">
         <v>123</v>
@@ -3863,7 +3872,7 @@
     </row>
     <row r="25" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B25" s="8" t="s">
         <v>124</v>
@@ -3877,7 +3886,7 @@
     </row>
     <row r="26" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B26" s="9" t="s">
         <v>125</v>
@@ -3892,10 +3901,10 @@
     </row>
     <row r="27" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C27" s="8" t="s">
         <v>126</v>
@@ -3909,7 +3918,7 @@
     </row>
     <row r="28" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B28" s="9" t="s">
         <v>127</v>
@@ -3930,7 +3939,7 @@
     </row>
     <row r="29" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B29" s="8" t="s">
         <v>128</v>
@@ -3962,13 +3971,13 @@
         <v>158</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C30" s="15" t="s">
+        <v>358</v>
+      </c>
+      <c r="D30" s="15" t="s">
         <v>359</v>
-      </c>
-      <c r="D30" s="15" t="s">
-        <v>360</v>
       </c>
       <c r="M30">
         <v>1</v>
@@ -4010,7 +4019,7 @@
     </row>
     <row r="31" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B31" s="8" t="s">
         <v>129</v>
@@ -4027,7 +4036,7 @@
     </row>
     <row r="32" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B32" s="9" t="s">
         <v>130</v>
@@ -4045,7 +4054,7 @@
     </row>
     <row r="33" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B33" s="8" t="s">
         <v>130</v>
@@ -4062,7 +4071,7 @@
     </row>
     <row r="34" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B34" s="9" t="s">
         <v>132</v>
@@ -4092,7 +4101,7 @@
     </row>
     <row r="35" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B35" s="8" t="s">
         <v>132</v>
@@ -4112,7 +4121,7 @@
     </row>
     <row r="36" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B36" s="9" t="s">
         <v>132</v>
@@ -4133,7 +4142,7 @@
     </row>
     <row r="37" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B37" s="8" t="s">
         <v>132</v>
@@ -4156,7 +4165,7 @@
     </row>
     <row r="38" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B38" s="9" t="s">
         <v>132</v>
@@ -4180,7 +4189,7 @@
     </row>
     <row r="39" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B39" s="8" t="s">
         <v>132</v>
@@ -4221,13 +4230,13 @@
     </row>
     <row r="40" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B40" s="9" t="s">
         <v>133</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D40" s="9" t="s">
         <v>172</v>
@@ -4239,13 +4248,13 @@
     </row>
     <row r="41" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B41" s="8" t="s">
         <v>133</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D41" s="8" t="s">
         <v>172</v>
@@ -4355,13 +4364,13 @@
     </row>
     <row r="42" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B42" s="9" t="s">
         <v>133</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D42" s="9" t="s">
         <v>172</v>
@@ -4382,13 +4391,13 @@
     </row>
     <row r="43" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A43" s="8" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B43" s="8" t="s">
         <v>133</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D43" s="8" t="s">
         <v>172</v>
@@ -4423,13 +4432,13 @@
     </row>
     <row r="44" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B44" s="9" t="s">
         <v>133</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D44" s="9" t="s">
         <v>172</v>
@@ -4447,13 +4456,13 @@
     </row>
     <row r="45" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A45" s="8" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B45" s="8" t="s">
         <v>133</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D45" s="8" t="s">
         <v>172</v>
@@ -4476,13 +4485,13 @@
     </row>
     <row r="46" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A46" s="9" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B46" s="9" t="s">
         <v>133</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D46" s="9" t="s">
         <v>172</v>
@@ -4509,13 +4518,13 @@
     </row>
     <row r="47" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A47" s="8" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B47" s="8" t="s">
         <v>133</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D47" s="8" t="s">
         <v>172</v>
@@ -4541,13 +4550,13 @@
     </row>
     <row r="48" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A48" s="9" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B48" s="9" t="s">
         <v>133</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D48" s="9" t="s">
         <v>172</v>
@@ -4559,13 +4568,13 @@
     </row>
     <row r="49" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A49" s="8" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B49" s="8" t="s">
         <v>133</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D49" s="8" t="s">
         <v>172</v>
@@ -4576,13 +4585,13 @@
     </row>
     <row r="50" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A50" s="9" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B50" s="9" t="s">
         <v>133</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D50" s="9" t="s">
         <v>172</v>
@@ -4597,13 +4606,13 @@
     </row>
     <row r="51" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A51" s="8" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B51" s="8" t="s">
         <v>133</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D51" s="8" t="s">
         <v>172</v>
@@ -4647,13 +4656,13 @@
     </row>
     <row r="52" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A52" s="9" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B52" s="9" t="s">
         <v>133</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D52" s="9" t="s">
         <v>172</v>
@@ -4779,13 +4788,13 @@
     </row>
     <row r="53" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A53" s="8" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B53" s="8" t="s">
         <v>133</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D53" s="8" t="s">
         <v>172</v>
@@ -4817,13 +4826,13 @@
     </row>
     <row r="54" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A54" s="9" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B54" s="9" t="s">
         <v>133</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D54" s="9" t="s">
         <v>172</v>
@@ -4901,13 +4910,13 @@
     </row>
     <row r="55" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A55" s="8" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B55" s="8" t="s">
         <v>133</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D55" s="8" t="s">
         <v>172</v>
@@ -4945,13 +4954,13 @@
     </row>
     <row r="56" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B56" s="9" t="s">
         <v>133</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D56" s="9" t="s">
         <v>172</v>
@@ -4963,13 +4972,13 @@
     </row>
     <row r="57" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A57" s="8" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B57" s="8" t="s">
         <v>133</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D57" s="8" t="s">
         <v>172</v>
@@ -5106,7 +5115,7 @@
     </row>
     <row r="58" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A58" s="9" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B58" s="9" t="s">
         <v>134</v>
@@ -5121,7 +5130,7 @@
     </row>
     <row r="59" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A59" s="8" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B59" s="8" t="s">
         <v>135</v>
@@ -5147,7 +5156,7 @@
     </row>
     <row r="60" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A60" s="9" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B60" s="9" t="s">
         <v>136</v>
@@ -5165,7 +5174,7 @@
     </row>
     <row r="61" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A61" s="8" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B61" s="8" t="s">
         <v>137</v>
@@ -5174,7 +5183,7 @@
         <v>138</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E61">
         <v>1</v>
@@ -5182,7 +5191,7 @@
     </row>
     <row r="62" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A62" s="9" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B62" s="9" t="s">
         <v>137</v>
@@ -5191,7 +5200,7 @@
         <v>138</v>
       </c>
       <c r="D62" s="9" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="N62">
         <v>1</v>
@@ -5206,7 +5215,7 @@
     </row>
     <row r="63" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A63" s="8" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B63" s="8" t="s">
         <v>137</v>
@@ -5215,7 +5224,7 @@
         <v>138</v>
       </c>
       <c r="D63" s="8" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="R63">
         <v>1</v>
@@ -5226,7 +5235,7 @@
     </row>
     <row r="64" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A64" s="9" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B64" s="9" t="s">
         <v>137</v>
@@ -5235,7 +5244,7 @@
         <v>138</v>
       </c>
       <c r="D64" s="9" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="AS64" s="10"/>
       <c r="CG64">
@@ -5247,7 +5256,7 @@
     </row>
     <row r="65" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A65" s="8" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B65" s="8" t="s">
         <v>137</v>
@@ -5256,7 +5265,7 @@
         <v>138</v>
       </c>
       <c r="D65" s="8" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="AU65">
         <v>1</v>
@@ -5264,7 +5273,7 @@
     </row>
     <row r="66" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A66" s="9" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B66" s="9" t="s">
         <v>137</v>
@@ -5273,7 +5282,7 @@
         <v>138</v>
       </c>
       <c r="D66" s="9" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="O66">
         <v>1</v>
@@ -5294,7 +5303,7 @@
     </row>
     <row r="67" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A67" s="8" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B67" s="8" t="s">
         <v>137</v>
@@ -5303,7 +5312,7 @@
         <v>138</v>
       </c>
       <c r="D67" s="8" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="AB67">
         <v>2</v>
@@ -5311,7 +5320,7 @@
     </row>
     <row r="68" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A68" s="9" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B68" s="9" t="s">
         <v>137</v>
@@ -5320,7 +5329,7 @@
         <v>138</v>
       </c>
       <c r="D68" s="9" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="M68">
         <v>1</v>
@@ -5347,7 +5356,7 @@
     </row>
     <row r="69" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A69" s="8" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B69" s="8" t="s">
         <v>137</v>
@@ -5356,7 +5365,7 @@
         <v>138</v>
       </c>
       <c r="D69" s="8" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="X69">
         <v>1</v>
@@ -5367,7 +5376,7 @@
     </row>
     <row r="70" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A70" s="9" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B70" s="9" t="s">
         <v>137</v>
@@ -5376,7 +5385,7 @@
         <v>138</v>
       </c>
       <c r="D70" s="9" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="AO70">
         <v>1</v>
@@ -5385,7 +5394,7 @@
     </row>
     <row r="71" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A71" s="8" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B71" s="8" t="s">
         <v>137</v>
@@ -5394,7 +5403,7 @@
         <v>138</v>
       </c>
       <c r="D71" s="8" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="CT71">
         <v>1</v>
@@ -5405,7 +5414,7 @@
     </row>
     <row r="72" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A72" s="9" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B72" s="17" t="s">
         <v>137</v>
@@ -5414,7 +5423,7 @@
         <v>138</v>
       </c>
       <c r="D72" s="9" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="Q72">
         <v>1</v>
@@ -5432,7 +5441,7 @@
     </row>
     <row r="73" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A73" s="8" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B73" s="8" t="s">
         <v>139</v>
@@ -5455,7 +5464,7 @@
     </row>
     <row r="74" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A74" s="9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B74" s="9" t="s">
         <v>139</v>
@@ -5473,7 +5482,7 @@
     </row>
     <row r="75" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A75" s="8" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B75" s="8" t="s">
         <v>139</v>
@@ -5496,7 +5505,7 @@
     </row>
     <row r="76" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A76" s="9" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B76" s="9" t="s">
         <v>140</v>
@@ -5511,7 +5520,7 @@
     </row>
     <row r="77" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A77" s="8" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B77" s="8" t="s">
         <v>141</v>
@@ -5525,7 +5534,7 @@
     </row>
     <row r="78" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A78" s="9" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B78" s="9" t="s">
         <v>142</v>
@@ -5534,13 +5543,13 @@
         <v>163</v>
       </c>
       <c r="D78" s="9" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="AS78" s="10"/>
     </row>
     <row r="79" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A79" s="8" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B79" s="8" t="s">
         <v>142</v>
@@ -5549,7 +5558,7 @@
         <v>163</v>
       </c>
       <c r="D79" s="8" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="DI79">
         <v>1</v>
@@ -5557,7 +5566,7 @@
     </row>
     <row r="80" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A80" s="9" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B80" s="9" t="s">
         <v>142</v>
@@ -5566,7 +5575,7 @@
         <v>163</v>
       </c>
       <c r="D80" s="9" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E80">
         <v>2</v>
@@ -5590,7 +5599,7 @@
     </row>
     <row r="81" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A81" s="8" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B81" s="8" t="s">
         <v>142</v>
@@ -5599,7 +5608,7 @@
         <v>163</v>
       </c>
       <c r="D81" s="8" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E81">
         <v>1</v>
@@ -5607,7 +5616,7 @@
     </row>
     <row r="82" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A82" s="9" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B82" s="9" t="s">
         <v>142</v>
@@ -5616,7 +5625,7 @@
         <v>163</v>
       </c>
       <c r="D82" s="9" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="AS82" s="10"/>
       <c r="DK82">
@@ -5625,7 +5634,7 @@
     </row>
     <row r="83" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A83" s="8" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B83" s="8" t="s">
         <v>142</v>
@@ -5634,7 +5643,7 @@
         <v>163</v>
       </c>
       <c r="D83" s="8" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="CQ83">
         <v>2</v>
@@ -5666,7 +5675,7 @@
     </row>
     <row r="84" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A84" s="9" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B84" s="9" t="s">
         <v>142</v>
@@ -5675,7 +5684,7 @@
         <v>163</v>
       </c>
       <c r="D84" s="9" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="Z84">
         <v>1</v>
@@ -5684,13 +5693,13 @@
     </row>
     <row r="85" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A85" s="8" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B85" s="15" t="s">
+        <v>351</v>
+      </c>
+      <c r="C85" s="15" t="s">
         <v>352</v>
-      </c>
-      <c r="C85" s="15" t="s">
-        <v>353</v>
       </c>
       <c r="D85" s="8" t="s">
         <v>143</v>
@@ -5701,7 +5710,7 @@
     </row>
     <row r="86" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A86" s="9" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B86" s="9" t="s">
         <v>145</v>
@@ -5710,7 +5719,7 @@
         <v>171</v>
       </c>
       <c r="D86" s="9" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="S86">
         <v>1</v>
@@ -5740,7 +5749,7 @@
     </row>
     <row r="87" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A87" s="8" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B87" s="8" t="s">
         <v>144</v>
@@ -5749,7 +5758,7 @@
         <v>171</v>
       </c>
       <c r="D87" s="8" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="DC87">
         <v>1</v>
@@ -5757,7 +5766,7 @@
     </row>
     <row r="88" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A88" s="9" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B88" s="9" t="s">
         <v>144</v>
@@ -5766,7 +5775,7 @@
         <v>171</v>
       </c>
       <c r="D88" s="9" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="AS88" s="10"/>
       <c r="CJ88">
@@ -5787,7 +5796,7 @@
     </row>
     <row r="89" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A89" s="8" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B89" s="8" t="s">
         <v>144</v>
@@ -5796,7 +5805,7 @@
         <v>171</v>
       </c>
       <c r="D89" s="8" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="CI89">
         <v>1</v>
@@ -5810,7 +5819,7 @@
     </row>
     <row r="90" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A90" s="9" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B90" s="9" t="s">
         <v>144</v>
@@ -5819,7 +5828,7 @@
         <v>171</v>
       </c>
       <c r="D90" s="9" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="AS90" s="10"/>
       <c r="CQ90">
@@ -5828,7 +5837,7 @@
     </row>
     <row r="91" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A91" s="8" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B91" s="8" t="s">
         <v>144</v>
@@ -5837,7 +5846,7 @@
         <v>171</v>
       </c>
       <c r="D91" s="8" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="CT91">
         <v>1</v>
@@ -5845,7 +5854,7 @@
     </row>
     <row r="92" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A92" s="9" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B92" s="9" t="s">
         <v>144</v>
@@ -5854,7 +5863,7 @@
         <v>171</v>
       </c>
       <c r="D92" s="9" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="AS92" s="10"/>
       <c r="CC92">
@@ -5863,7 +5872,7 @@
     </row>
     <row r="93" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A93" s="8" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B93" s="8" t="s">
         <v>144</v>
@@ -5872,7 +5881,7 @@
         <v>171</v>
       </c>
       <c r="D93" s="8" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="BN93">
         <v>1</v>
@@ -5889,7 +5898,7 @@
     </row>
     <row r="94" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A94" s="9" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B94" s="9" t="s">
         <v>144</v>
@@ -5898,7 +5907,7 @@
         <v>171</v>
       </c>
       <c r="D94" s="9" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="AS94" s="10"/>
       <c r="CI94">
@@ -5913,7 +5922,7 @@
     </row>
     <row r="95" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A95" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B95" s="8" t="s">
         <v>144</v>
@@ -5922,7 +5931,7 @@
         <v>171</v>
       </c>
       <c r="D95" s="8" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="CA95">
         <v>1</v>
@@ -5936,7 +5945,7 @@
     </row>
     <row r="96" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A96" s="9" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B96" s="9" t="s">
         <v>144</v>
@@ -5945,7 +5954,7 @@
         <v>171</v>
       </c>
       <c r="D96" s="9" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="AS96" s="10"/>
       <c r="CW96">
@@ -5957,7 +5966,7 @@
     </row>
     <row r="97" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A97" s="8" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B97" s="8" t="s">
         <v>144</v>
@@ -5966,7 +5975,7 @@
         <v>171</v>
       </c>
       <c r="D97" s="8" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="M97">
         <v>1</v>
@@ -6019,7 +6028,7 @@
     </row>
     <row r="98" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A98" s="9" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B98" s="9" t="s">
         <v>144</v>
@@ -6028,7 +6037,7 @@
         <v>171</v>
       </c>
       <c r="D98" s="9" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="AS98" s="10"/>
       <c r="CY98">
@@ -6040,7 +6049,7 @@
     </row>
     <row r="99" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A99" s="8" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B99" s="8" t="s">
         <v>144</v>
@@ -6049,7 +6058,7 @@
         <v>171</v>
       </c>
       <c r="D99" s="8" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="DN99">
         <v>2</v>
@@ -6057,7 +6066,7 @@
     </row>
     <row r="100" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A100" s="9" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B100" s="9" t="s">
         <v>144</v>
@@ -6066,7 +6075,7 @@
         <v>171</v>
       </c>
       <c r="D100" s="9" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="AS100" s="10"/>
       <c r="BZ100">
@@ -6078,7 +6087,7 @@
     </row>
     <row r="101" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A101" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B101" s="8" t="s">
         <v>144</v>
@@ -6087,7 +6096,7 @@
         <v>171</v>
       </c>
       <c r="D101" s="8" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="BQ101">
         <v>1</v>
@@ -6104,7 +6113,7 @@
     </row>
     <row r="102" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A102" s="9" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B102" s="9" t="s">
         <v>144</v>
@@ -6113,7 +6122,7 @@
         <v>171</v>
       </c>
       <c r="D102" s="9" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="AS102" s="10"/>
       <c r="BP102">
@@ -6143,7 +6152,7 @@
     </row>
     <row r="103" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A103" s="8" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B103" s="8" t="s">
         <v>144</v>
@@ -6152,7 +6161,7 @@
         <v>171</v>
       </c>
       <c r="D103" s="8" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="CB103">
         <v>1</v>
@@ -6163,7 +6172,7 @@
     </row>
     <row r="104" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A104" s="9" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B104" s="9" t="s">
         <v>144</v>
@@ -6172,7 +6181,7 @@
         <v>171</v>
       </c>
       <c r="D104" s="9" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="S104">
         <v>1</v>
@@ -6226,7 +6235,7 @@
     </row>
     <row r="105" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A105" s="8" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B105" s="8" t="s">
         <v>144</v>
@@ -6235,7 +6244,7 @@
         <v>171</v>
       </c>
       <c r="D105" s="8" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="BS105">
         <v>1</v>
@@ -6243,7 +6252,7 @@
     </row>
     <row r="106" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A106" s="9" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B106" s="9" t="s">
         <v>144</v>
@@ -6252,7 +6261,7 @@
         <v>171</v>
       </c>
       <c r="D106" s="9" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="AS106" s="10"/>
       <c r="CE106">
@@ -6261,7 +6270,7 @@
     </row>
     <row r="107" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A107" s="8" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B107" s="8" t="s">
         <v>144</v>
@@ -6270,7 +6279,7 @@
         <v>171</v>
       </c>
       <c r="D107" s="8" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="F107">
         <v>1</v>
@@ -6302,7 +6311,7 @@
     </row>
     <row r="108" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A108" s="9" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B108" s="9" t="s">
         <v>144</v>
@@ -6311,7 +6320,7 @@
         <v>171</v>
       </c>
       <c r="D108" s="9" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="AS108" s="10"/>
       <c r="DI108">
@@ -6332,7 +6341,7 @@
     </row>
     <row r="109" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A109" s="8" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B109" s="8" t="s">
         <v>144</v>
@@ -6341,7 +6350,7 @@
         <v>171</v>
       </c>
       <c r="D109" s="8" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="J109">
         <v>1</v>
@@ -6349,7 +6358,7 @@
     </row>
     <row r="110" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A110" s="9" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B110" s="9" t="s">
         <v>144</v>
@@ -6358,7 +6367,7 @@
         <v>171</v>
       </c>
       <c r="D110" s="9" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="AS110" s="10"/>
       <c r="DN110">
@@ -6367,7 +6376,7 @@
     </row>
     <row r="111" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A111" s="8" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B111" s="8" t="s">
         <v>144</v>
@@ -6376,7 +6385,7 @@
         <v>171</v>
       </c>
       <c r="D111" s="8" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="CZ111">
         <v>1</v>
@@ -6387,7 +6396,7 @@
     </row>
     <row r="112" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A112" s="9" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B112" s="9" t="s">
         <v>144</v>
@@ -6396,7 +6405,7 @@
         <v>171</v>
       </c>
       <c r="D112" s="9" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="O112">
         <v>1</v>
@@ -6447,7 +6456,7 @@
     </row>
     <row r="113" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A113" s="8" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B113" s="8" t="s">
         <v>144</v>
@@ -6476,7 +6485,7 @@
     </row>
     <row r="114" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A114" s="9" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B114" s="9" t="s">
         <v>144</v>
@@ -6485,7 +6494,7 @@
         <v>171</v>
       </c>
       <c r="D114" s="9" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="AS114" s="10"/>
       <c r="CA114">
@@ -6506,7 +6515,7 @@
     </row>
     <row r="115" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A115" s="8" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B115" s="8" t="s">
         <v>144</v>
@@ -6559,7 +6568,7 @@
     </row>
     <row r="116" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A116" s="9" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B116" s="9" t="s">
         <v>144</v>
@@ -6568,7 +6577,7 @@
         <v>171</v>
       </c>
       <c r="D116" s="9" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="AS116" s="10"/>
       <c r="DS116">
@@ -6577,7 +6586,7 @@
     </row>
     <row r="117" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A117" s="8" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B117" s="8" t="s">
         <v>144</v>
@@ -6586,7 +6595,7 @@
         <v>171</v>
       </c>
       <c r="D117" s="8" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="CU117">
         <v>1</v>
@@ -6603,7 +6612,7 @@
     </row>
     <row r="118" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A118" s="9" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B118" s="9" t="s">
         <v>144</v>
@@ -6612,7 +6621,7 @@
         <v>171</v>
       </c>
       <c r="D118" s="9" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="S118">
         <v>1</v>
@@ -6633,7 +6642,7 @@
     </row>
     <row r="119" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A119" s="8" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B119" s="8" t="s">
         <v>144</v>
@@ -6642,7 +6651,7 @@
         <v>171</v>
       </c>
       <c r="D119" s="8" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="CH119">
         <v>1</v>
@@ -6653,7 +6662,7 @@
     </row>
     <row r="120" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A120" s="9" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B120" s="9" t="s">
         <v>144</v>
@@ -6662,7 +6671,7 @@
         <v>171</v>
       </c>
       <c r="D120" s="9" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="AS120" s="10"/>
       <c r="CV120">
@@ -6674,7 +6683,7 @@
     </row>
     <row r="121" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A121" s="8" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B121" s="8" t="s">
         <v>144</v>
@@ -6683,7 +6692,7 @@
         <v>171</v>
       </c>
       <c r="D121" s="8" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="CH121">
         <v>1</v>
@@ -6697,7 +6706,7 @@
     </row>
     <row r="122" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A122" s="8" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B122" s="8" t="s">
         <v>145</v>
@@ -6706,7 +6715,7 @@
         <v>171</v>
       </c>
       <c r="D122" s="8" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="BK122">
         <v>2</v>
@@ -6765,13 +6774,13 @@
     </row>
     <row r="123" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A123" s="9" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B123" s="9" t="s">
         <v>146</v>
       </c>
       <c r="C123" s="9" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="D123" s="9" t="s">
         <v>160</v>
@@ -6795,13 +6804,13 @@
     </row>
     <row r="124" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A124" s="8" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B124" s="8" t="s">
         <v>147</v>
       </c>
       <c r="C124" s="8" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D124" s="8" t="s">
         <v>160</v>
@@ -6812,7 +6821,7 @@
     </row>
     <row r="125" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A125" s="9" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B125" s="9" t="s">
         <v>148</v>
@@ -6836,7 +6845,7 @@
     </row>
     <row r="126" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A126" s="8" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B126" s="8" t="s">
         <v>149</v>
@@ -6856,13 +6865,13 @@
         <v>107</v>
       </c>
       <c r="B127" s="15" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C127" s="15" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D127" s="9" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="M127">
         <v>2</v>
@@ -6871,7 +6880,7 @@
     </row>
     <row r="128" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A128" s="8" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B128" s="8" t="s">
         <v>150</v>
@@ -6880,7 +6889,7 @@
         <v>195</v>
       </c>
       <c r="D128" s="8" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="DV128">
         <v>1</v>
@@ -6894,7 +6903,7 @@
     </row>
     <row r="129" spans="1:128" x14ac:dyDescent="0.25">
       <c r="A129" s="9" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B129" s="9" t="s">
         <v>150</v>
@@ -6903,7 +6912,7 @@
         <v>195</v>
       </c>
       <c r="D129" s="9" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="AS129" s="10"/>
       <c r="DV129">
@@ -6912,7 +6921,7 @@
     </row>
     <row r="130" spans="1:128" x14ac:dyDescent="0.25">
       <c r="A130" s="8" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B130" s="8" t="s">
         <v>150</v>
@@ -6921,7 +6930,7 @@
         <v>195</v>
       </c>
       <c r="D130" s="8" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="CK130">
         <v>1</v>
@@ -6938,7 +6947,7 @@
     </row>
     <row r="131" spans="1:128" x14ac:dyDescent="0.25">
       <c r="A131" s="9" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B131" s="9" t="s">
         <v>150</v>
@@ -6947,7 +6956,7 @@
         <v>195</v>
       </c>
       <c r="D131" s="9" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="S131">
         <v>4</v>
@@ -6965,7 +6974,7 @@
     </row>
     <row r="132" spans="1:128" x14ac:dyDescent="0.25">
       <c r="A132" s="8" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B132" s="8" t="s">
         <v>151</v>
@@ -6982,22 +6991,22 @@
     </row>
     <row r="133" spans="1:128" x14ac:dyDescent="0.25">
       <c r="A133" s="9" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B133" s="15" t="s">
+        <v>355</v>
+      </c>
+      <c r="C133" s="15" t="s">
         <v>356</v>
       </c>
-      <c r="C133" s="15" t="s">
+      <c r="D133" s="15" t="s">
         <v>357</v>
-      </c>
-      <c r="D133" s="15" t="s">
-        <v>358</v>
       </c>
       <c r="AS133" s="10"/>
     </row>
     <row r="134" spans="1:128" x14ac:dyDescent="0.25">
       <c r="A134" s="8" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B134" s="8" t="s">
         <v>152</v>
@@ -7014,7 +7023,7 @@
     </row>
     <row r="135" spans="1:128" x14ac:dyDescent="0.25">
       <c r="A135" s="9" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B135" s="9" t="s">
         <v>153</v>
@@ -7035,16 +7044,16 @@
     </row>
     <row r="136" spans="1:128" x14ac:dyDescent="0.25">
       <c r="A136" s="8" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B136" s="8" t="s">
         <v>154</v>
       </c>
       <c r="C136" s="14" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D136" s="8" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="AX136">
         <v>1</v>
@@ -7058,7 +7067,7 @@
     </row>
     <row r="137" spans="1:128" x14ac:dyDescent="0.25">
       <c r="A137" s="9" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B137" s="9" t="s">
         <v>155</v>
@@ -7067,7 +7076,7 @@
         <v>196</v>
       </c>
       <c r="D137" s="9" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="Q137">
         <v>1</v>
@@ -7079,7 +7088,7 @@
     </row>
     <row r="138" spans="1:128" x14ac:dyDescent="0.25">
       <c r="A138" s="8" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B138" s="8" t="s">
         <v>156</v>
@@ -7093,7 +7102,7 @@
     </row>
     <row r="139" spans="1:128" x14ac:dyDescent="0.25">
       <c r="A139" s="9" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B139" s="9" t="s">
         <v>157</v>
@@ -7102,7 +7111,7 @@
         <v>197</v>
       </c>
       <c r="D139" s="9" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="AS139" s="10"/>
       <c r="BJ139">

</xml_diff>

<commit_message>
removing old version of files
</commit_message>
<xml_diff>
--- a/Data/data_sour_rot.xlsx
+++ b/Data/data_sour_rot.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\U80821784\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{028BBA51-D238-4642-8A4F-A2CA22065A2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D15933C-CA33-4309-9768-5CE513958566}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -2580,7 +2580,9 @@
   <dimension ref="A1:DY139"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection activeCell="A97" sqref="A97"/>
+      <selection pane="topRight" activeCell="B146" sqref="B146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>

</xml_diff>